<commit_message>
Fix concerns of miss maylen in JO
</commit_message>
<xml_diff>
--- a/JOR Summary.xlsx
+++ b/JOR Summary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>JOR Summary 2021</t>
   </si>
@@ -89,67 +89,82 @@
     <t>End User's Comments</t>
   </si>
   <si>
-    <t>2021-08-24</t>
-  </si>
-  <si>
-    <t>2021-08-26</t>
-  </si>
-  <si>
-    <t>BCD</t>
-  </si>
-  <si>
-    <t>Repair of entrance front door glass.</t>
-  </si>
-  <si>
-    <t>JOR 2021-1-CNPR</t>
-  </si>
-  <si>
-    <t>Syndey Sinoro</t>
+    <t>2021-09-08</t>
+  </si>
+  <si>
+    <t>2021-09-11</t>
+  </si>
+  <si>
+    <t>CNPR-S</t>
+  </si>
+  <si>
+    <t>INSTALLATION OF ADDITIONAL CCTV CAMERA IN DRAIN CANALS AND LADIES DORM</t>
+  </si>
+  <si>
+    <t>JOR 2021-1-CNPR / CNPR-S-EMG-9821-1002</t>
+  </si>
+  <si>
+    <t>GODFREY SAMANO</t>
   </si>
   <si>
     <t xml:space="preserve">
 </t>
   </si>
   <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item no. 1 sample </t>
-  </si>
-  <si>
-    <t>Testing Offer</t>
-  </si>
-  <si>
-    <t>Testing jashdk jka sdjk
-klsajdl k</t>
-  </si>
-  <si>
-    <t>Partially Delivered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item no. 2 sample </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JO AOQ Done - For TE - 2021-09-03
+    <t>lot/s</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Materials &amp; Equipment preparations. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For JO - AOQ Done (awarded) 
 </t>
   </si>
   <si>
     <t>Pending</t>
   </si>
   <si>
-    <t xml:space="preserve">Item no. 3 sample </t>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lay-out &amp; excavation of underground pathway </t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
-    <t xml:space="preserve">Item no. 4 sample </t>
-  </si>
-  <si>
-    <t>aragay nars</t>
+    <t xml:space="preserve">Excavation of pole foundation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For RFQ 
+</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erection of steel pole </t>
+  </si>
+  <si>
+    <t>Testing lng danay ah</t>
   </si>
   <si>
     <t>JO Issued</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistance in cable pulling &amp; laying of conduit pipe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backfilling &amp; compaction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hauling of materials &amp; housekeeping </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accomplish the attached Excavation Specification </t>
   </si>
 </sst>
 </file>
@@ -186,19 +201,13 @@
       <name val="Arial Black"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFf7ffb9"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -229,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="16">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -242,6 +251,24 @@
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -258,42 +285,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -595,10 +586,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="V8" sqref="V8"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -609,19 +600,19 @@
     <col min="4" max="4" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="43.560791" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="18.709717" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="5.855713" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="83.693848" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="45.845947" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="17.567139" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="5.855713" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="22.280273" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="18.709717" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="63.555908" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="24.708252" bestFit="true" customWidth="true" style="0"/>
     <col min="16" max="16" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="39.990234" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="23.422852" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="34.134521" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="11.711426" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="9.283447" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="17.567139" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="23.422852" bestFit="true" customWidth="true" style="0"/>
@@ -734,7 +725,7 @@
         <v>29</v>
       </c>
       <c r="J5" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>30</v>
@@ -742,19 +733,15 @@
       <c r="L5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="4"/>
+      <c r="M5" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="N5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="O5" s="8"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
       <c r="R5" s="9" t="s">
         <v>34</v>
       </c>
@@ -766,160 +753,370 @@
       <c r="V5" s="5"/>
     </row>
     <row r="6" spans="1:22">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="12">
-        <v>1</v>
-      </c>
-      <c r="K6" s="12" t="s">
+      <c r="J6" s="6">
+        <v>10</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="10"/>
-      <c r="N6" s="13" t="s">
+      <c r="L6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="O6" s="14"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="15" t="s">
+      <c r="M6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="S6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
     </row>
     <row r="7" spans="1:22">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="11" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="12">
-        <v>1</v>
-      </c>
-      <c r="K7" s="12" t="s">
+      <c r="J7" s="6">
+        <v>2</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="13" t="s">
+      <c r="L7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="O7" s="14"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="S7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
     </row>
     <row r="8" spans="1:22">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="17" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="18">
-        <v>1</v>
-      </c>
-      <c r="K8" s="18" t="s">
+      <c r="J8" s="12">
+        <v>20</v>
+      </c>
+      <c r="K8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="16" t="s">
+      <c r="L8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="P8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="12">
+        <v>5</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="12">
+        <v>3</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="P10" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="6">
+        <v>5</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="4"/>
+      <c r="N11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O11" s="8"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="6">
+        <v>3</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="M12" s="4"/>
+      <c r="N12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="8"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="O8" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="P8" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="R8" s="21"/>
-      <c r="S8" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
+      <c r="S12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>